<commit_message>
iteration 3 player 0
</commit_message>
<xml_diff>
--- a/tests/src/blueprint/human strategy.xlsx
+++ b/tests/src/blueprint/human strategy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marzukrashid/Downloads/fishbait/fishbait/tests/src/blueprint/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD59AAF-A3D2-3047-A83B-283D61323AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1A2C1C-2224-DB49-A59E-7DED97577F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -652,7 +652,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -865,6 +865,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2032,7 +2038,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J78" sqref="J78"/>
+      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2149,14 +2155,14 @@
       <c r="A3" s="7">
         <v>0</v>
       </c>
-      <c r="B3" s="41">
-        <v>0</v>
-      </c>
-      <c r="C3" s="28">
-        <v>0</v>
-      </c>
-      <c r="D3" s="28">
-        <v>0</v>
+      <c r="B3" s="71">
+        <v>5017</v>
+      </c>
+      <c r="C3" s="72">
+        <v>-4983</v>
+      </c>
+      <c r="D3" s="72">
+        <v>-33</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="46"/>
@@ -3132,11 +3138,11 @@
       <c r="D26" s="61"/>
       <c r="E26" s="62"/>
       <c r="F26" s="50"/>
-      <c r="G26" s="42">
-        <v>0</v>
-      </c>
-      <c r="H26" s="31">
-        <v>0</v>
+      <c r="G26" s="60">
+        <v>4950</v>
+      </c>
+      <c r="H26" s="61">
+        <v>-4950</v>
       </c>
       <c r="I26" s="31"/>
       <c r="J26" s="14"/>
@@ -6877,10 +6883,10 @@
   <dimension ref="A1:P104"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B73" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B89" sqref="B89"/>
+      <selection pane="bottomRight" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
strategy test iteration 3 player 1
</commit_message>
<xml_diff>
--- a/tests/src/blueprint/human strategy.xlsx
+++ b/tests/src/blueprint/human strategy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marzukrashid/Downloads/fishbait/fishbait/tests/src/blueprint/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1A2C1C-2224-DB49-A59E-7DED97577F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC27102B-9157-C44F-916A-6C13C1218583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -125,12 +125,14 @@
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -652,7 +654,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -845,6 +847,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -866,10 +874,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2038,7 +2049,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomRight" activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2057,34 +2068,34 @@
   <sheetData>
     <row r="1" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2"/>
-      <c r="B1" s="64">
-        <v>0</v>
-      </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="67">
-        <v>1</v>
-      </c>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="67">
-        <v>2</v>
-      </c>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="66"/>
-      <c r="Q1" s="67">
+      <c r="B1" s="66">
+        <v>0</v>
+      </c>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="69">
+        <v>1</v>
+      </c>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="69">
+        <v>2</v>
+      </c>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="68"/>
+      <c r="Q1" s="69">
         <v>3</v>
       </c>
-      <c r="R1" s="65"/>
-      <c r="S1" s="65"/>
-      <c r="T1" s="65"/>
-      <c r="U1" s="66"/>
+      <c r="R1" s="67"/>
+      <c r="S1" s="67"/>
+      <c r="T1" s="67"/>
+      <c r="U1" s="68"/>
     </row>
     <row r="2" spans="1:21" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
@@ -2155,13 +2166,13 @@
       <c r="A3" s="7">
         <v>0</v>
       </c>
-      <c r="B3" s="71">
+      <c r="B3" s="64">
         <v>5017</v>
       </c>
-      <c r="C3" s="72">
+      <c r="C3" s="65">
         <v>-4983</v>
       </c>
-      <c r="D3" s="72">
+      <c r="D3" s="65">
         <v>-33</v>
       </c>
       <c r="E3" s="9"/>
@@ -2218,25 +2229,25 @@
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="47"/>
-      <c r="G4" s="42">
-        <v>0</v>
-      </c>
-      <c r="H4" s="31">
-        <v>0</v>
-      </c>
-      <c r="I4" s="31">
+      <c r="G4" s="60">
+        <v>0</v>
+      </c>
+      <c r="H4" s="61">
+        <v>0</v>
+      </c>
+      <c r="I4" s="61">
         <v>0</v>
       </c>
       <c r="J4" s="14"/>
       <c r="K4" s="47"/>
-      <c r="L4" s="42">
-        <v>0</v>
-      </c>
-      <c r="M4" s="31">
-        <v>0</v>
-      </c>
-      <c r="N4" s="31">
-        <v>0</v>
+      <c r="L4" s="60">
+        <v>2458</v>
+      </c>
+      <c r="M4" s="61">
+        <v>-7492</v>
+      </c>
+      <c r="N4" s="61">
+        <v>5033</v>
       </c>
       <c r="O4" s="14"/>
       <c r="P4" s="47"/>
@@ -2934,19 +2945,19 @@
       <c r="E21" s="23"/>
       <c r="F21" s="49"/>
       <c r="G21" s="44"/>
-      <c r="H21" s="37">
-        <v>0</v>
-      </c>
-      <c r="I21" s="37">
-        <v>0</v>
+      <c r="H21" s="75">
+        <v>-2425</v>
+      </c>
+      <c r="I21" s="75">
+        <v>2425</v>
       </c>
       <c r="J21" s="23"/>
       <c r="K21" s="49"/>
       <c r="L21" s="53"/>
-      <c r="M21" s="23">
-        <v>0</v>
-      </c>
-      <c r="N21" s="23">
+      <c r="M21" s="74">
+        <v>0</v>
+      </c>
+      <c r="N21" s="74">
         <v>0</v>
       </c>
       <c r="O21" s="23"/>
@@ -3056,19 +3067,19 @@
       <c r="D24" s="31"/>
       <c r="E24" s="14"/>
       <c r="F24" s="50"/>
-      <c r="G24" s="42">
-        <v>0</v>
-      </c>
-      <c r="H24" s="31">
-        <v>0</v>
+      <c r="G24" s="60">
+        <v>-5050</v>
+      </c>
+      <c r="H24" s="61">
+        <v>5050</v>
       </c>
       <c r="I24" s="31"/>
       <c r="J24" s="14"/>
       <c r="K24" s="50"/>
-      <c r="L24" s="54">
-        <v>0</v>
-      </c>
-      <c r="M24" s="14">
+      <c r="L24" s="73">
+        <v>0</v>
+      </c>
+      <c r="M24" s="62">
         <v>0</v>
       </c>
       <c r="N24" s="14"/>
@@ -6473,44 +6484,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="68" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
+      <c r="A1" s="70" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
     </row>
     <row r="2" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3"/>
-      <c r="B2" s="64">
-        <v>0</v>
-      </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="70">
-        <v>1</v>
-      </c>
-      <c r="F2" s="65"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="70">
-        <v>2</v>
-      </c>
-      <c r="I2" s="65"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="70">
+      <c r="B2" s="66">
+        <v>0</v>
+      </c>
+      <c r="C2" s="67"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="72">
+        <v>1</v>
+      </c>
+      <c r="F2" s="67"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="72">
+        <v>2</v>
+      </c>
+      <c r="I2" s="67"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="72">
         <v>3</v>
       </c>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
     </row>
     <row r="3" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
@@ -6886,7 +6897,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C26" sqref="C26"/>
+      <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6896,24 +6907,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="68" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
+      <c r="A1" s="70" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
+      <c r="N1" s="70"/>
+      <c r="O1" s="70"/>
+      <c r="P1" s="70"/>
     </row>
     <row r="2" spans="1:16" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
@@ -11836,7 +11847,7 @@
     <mergeCell ref="A1:P1"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup scale="29" orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
strategy test fix regret max
</commit_message>
<xml_diff>
--- a/tests/src/blueprint/human strategy.xlsx
+++ b/tests/src/blueprint/human strategy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marzukrashid/Downloads/fishbait/fishbait/tests/src/blueprint/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC27102B-9157-C44F-916A-6C13C1218583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7287039-2040-AC4E-B003-0C73288F72DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="regrets" sheetId="1" r:id="rId1"/>
@@ -853,6 +853,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -873,15 +882,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2049,7 +2049,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J15" sqref="J15"/>
+      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2068,34 +2068,34 @@
   <sheetData>
     <row r="1" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2"/>
-      <c r="B1" s="66">
-        <v>0</v>
-      </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="69">
-        <v>1</v>
-      </c>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="69">
-        <v>2</v>
-      </c>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="69">
+      <c r="B1" s="69">
+        <v>0</v>
+      </c>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="72">
+        <v>1</v>
+      </c>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="72">
+        <v>2</v>
+      </c>
+      <c r="M1" s="70"/>
+      <c r="N1" s="70"/>
+      <c r="O1" s="70"/>
+      <c r="P1" s="71"/>
+      <c r="Q1" s="72">
         <v>3</v>
       </c>
-      <c r="R1" s="67"/>
-      <c r="S1" s="67"/>
-      <c r="T1" s="67"/>
-      <c r="U1" s="68"/>
+      <c r="R1" s="70"/>
+      <c r="S1" s="70"/>
+      <c r="T1" s="70"/>
+      <c r="U1" s="71"/>
     </row>
     <row r="2" spans="1:21" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
@@ -2945,19 +2945,19 @@
       <c r="E21" s="23"/>
       <c r="F21" s="49"/>
       <c r="G21" s="44"/>
-      <c r="H21" s="75">
+      <c r="H21" s="68">
         <v>-2425</v>
       </c>
-      <c r="I21" s="75">
+      <c r="I21" s="68">
         <v>2425</v>
       </c>
       <c r="J21" s="23"/>
       <c r="K21" s="49"/>
       <c r="L21" s="53"/>
-      <c r="M21" s="74">
-        <v>0</v>
-      </c>
-      <c r="N21" s="74">
+      <c r="M21" s="67">
+        <v>0</v>
+      </c>
+      <c r="N21" s="67">
         <v>0</v>
       </c>
       <c r="O21" s="23"/>
@@ -3076,7 +3076,7 @@
       <c r="I24" s="31"/>
       <c r="J24" s="14"/>
       <c r="K24" s="50"/>
-      <c r="L24" s="73">
+      <c r="L24" s="66">
         <v>0</v>
       </c>
       <c r="M24" s="62">
@@ -6484,44 +6484,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="70" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
+      <c r="A1" s="73" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
     </row>
     <row r="2" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3"/>
-      <c r="B2" s="66">
-        <v>0</v>
-      </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="72">
-        <v>1</v>
-      </c>
-      <c r="F2" s="67"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="72">
-        <v>2</v>
-      </c>
-      <c r="I2" s="67"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="72">
+      <c r="B2" s="69">
+        <v>0</v>
+      </c>
+      <c r="C2" s="70"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="75">
+        <v>1</v>
+      </c>
+      <c r="F2" s="70"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="75">
+        <v>2</v>
+      </c>
+      <c r="I2" s="70"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="75">
         <v>3</v>
       </c>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
     </row>
     <row r="3" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
@@ -6907,24 +6907,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="70" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
+      <c r="A1" s="73" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
     </row>
     <row r="2" spans="1:16" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">

</xml_diff>

<commit_message>
iteration 3 player 2
</commit_message>
<xml_diff>
--- a/tests/src/blueprint/human strategy.xlsx
+++ b/tests/src/blueprint/human strategy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marzukrashid/Downloads/fishbait/fishbait/tests/src/blueprint/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7287039-2040-AC4E-B003-0C73288F72DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5755BE0-14AF-D743-8C7E-1C8A20E507C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2046,10 +2046,10 @@
   <dimension ref="A1:U104"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
+      <selection pane="bottomRight" activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6897,7 +6897,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
strategy test iteration 4 player 0 update strategy
</commit_message>
<xml_diff>
--- a/tests/src/blueprint/human strategy.xlsx
+++ b/tests/src/blueprint/human strategy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marzukrashid/Downloads/fishbait/fishbait/tests/src/blueprint/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5755BE0-14AF-D743-8C7E-1C8A20E507C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639EBAC5-474A-9446-BFBA-E4AE346B18A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="regrets" sheetId="1" r:id="rId1"/>
@@ -2045,11 +2045,11 @@
   </sheetPr>
   <dimension ref="A1:U104"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M6" sqref="M6"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6474,7 +6474,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6568,51 +6568,115 @@
       <c r="A4" s="7">
         <v>0</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
+      <c r="B4" s="8">
+        <v>0</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0</v>
+      </c>
+      <c r="E4" s="11">
+        <v>0</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0</v>
+      </c>
+      <c r="G4" s="10">
+        <v>0</v>
+      </c>
+      <c r="H4" s="11">
+        <v>0</v>
+      </c>
+      <c r="I4" s="9">
+        <v>0</v>
+      </c>
+      <c r="J4" s="10">
+        <v>0</v>
+      </c>
+      <c r="K4" s="11">
+        <v>1</v>
+      </c>
+      <c r="L4" s="9">
+        <v>0</v>
+      </c>
+      <c r="M4" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="12">
         <v>1</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
+      <c r="B5" s="13">
+        <v>0</v>
+      </c>
+      <c r="C5" s="14">
+        <v>0</v>
+      </c>
+      <c r="D5" s="15">
+        <v>0</v>
+      </c>
+      <c r="E5" s="16">
+        <v>0</v>
+      </c>
+      <c r="F5" s="14">
+        <v>0</v>
+      </c>
+      <c r="G5" s="15">
+        <v>0</v>
+      </c>
+      <c r="H5" s="16">
+        <v>0</v>
+      </c>
+      <c r="I5" s="14">
+        <v>0</v>
+      </c>
+      <c r="J5" s="15">
+        <v>0</v>
+      </c>
+      <c r="K5" s="16">
+        <v>0</v>
+      </c>
+      <c r="L5" s="14">
+        <v>0</v>
+      </c>
+      <c r="M5" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="12">
         <v>2</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="14"/>
+      <c r="B6" s="13">
+        <v>0</v>
+      </c>
+      <c r="C6" s="14">
+        <v>0</v>
+      </c>
       <c r="D6" s="15"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="14"/>
+      <c r="E6" s="16">
+        <v>0</v>
+      </c>
+      <c r="F6" s="14">
+        <v>0</v>
+      </c>
       <c r="G6" s="15"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="14"/>
+      <c r="H6" s="16">
+        <v>0</v>
+      </c>
+      <c r="I6" s="14">
+        <v>0</v>
+      </c>
       <c r="J6" s="15"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="14"/>
+      <c r="K6" s="16">
+        <v>0</v>
+      </c>
+      <c r="L6" s="14">
+        <v>0</v>
+      </c>
       <c r="M6" s="14"/>
     </row>
     <row r="7" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -6620,186 +6684,370 @@
         <v>3</v>
       </c>
       <c r="B7" s="13"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="15"/>
+      <c r="C7" s="14">
+        <v>0</v>
+      </c>
+      <c r="D7" s="15">
+        <v>0</v>
+      </c>
       <c r="E7" s="16"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="15"/>
+      <c r="F7" s="14">
+        <v>0</v>
+      </c>
+      <c r="G7" s="15">
+        <v>0</v>
+      </c>
       <c r="H7" s="16"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="15"/>
+      <c r="I7" s="14">
+        <v>0</v>
+      </c>
+      <c r="J7" s="15">
+        <v>0</v>
+      </c>
       <c r="K7" s="16"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
+      <c r="L7" s="14">
+        <v>0</v>
+      </c>
+      <c r="M7" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="12">
         <v>4</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
+      <c r="B8" s="13">
+        <v>0</v>
+      </c>
+      <c r="C8" s="14">
+        <v>0</v>
+      </c>
       <c r="D8" s="15"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="14"/>
+      <c r="E8" s="16">
+        <v>0</v>
+      </c>
+      <c r="F8" s="14">
+        <v>0</v>
+      </c>
       <c r="G8" s="15"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="14"/>
+      <c r="H8" s="16">
+        <v>0</v>
+      </c>
+      <c r="I8" s="14">
+        <v>0</v>
+      </c>
       <c r="J8" s="15"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="14"/>
+      <c r="K8" s="16">
+        <v>0</v>
+      </c>
+      <c r="L8" s="14">
+        <v>0</v>
+      </c>
       <c r="M8" s="14"/>
     </row>
     <row r="9" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="12">
         <v>5</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="14"/>
+      <c r="B9" s="13">
+        <v>0</v>
+      </c>
+      <c r="C9" s="14">
+        <v>0</v>
+      </c>
       <c r="D9" s="15"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="14"/>
+      <c r="E9" s="16">
+        <v>0</v>
+      </c>
+      <c r="F9" s="14">
+        <v>0</v>
+      </c>
       <c r="G9" s="15"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="14"/>
+      <c r="H9" s="16">
+        <v>0</v>
+      </c>
+      <c r="I9" s="14">
+        <v>0</v>
+      </c>
       <c r="J9" s="15"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="14"/>
+      <c r="K9" s="16">
+        <v>0</v>
+      </c>
+      <c r="L9" s="14">
+        <v>0</v>
+      </c>
       <c r="M9" s="14"/>
     </row>
     <row r="10" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="12">
         <v>6</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="14"/>
+      <c r="B10" s="13">
+        <v>0</v>
+      </c>
+      <c r="C10" s="14">
+        <v>0</v>
+      </c>
       <c r="D10" s="15"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="14"/>
+      <c r="E10" s="16">
+        <v>0</v>
+      </c>
+      <c r="F10" s="14">
+        <v>0</v>
+      </c>
       <c r="G10" s="15"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="14"/>
+      <c r="H10" s="16">
+        <v>0</v>
+      </c>
+      <c r="I10" s="14">
+        <v>0</v>
+      </c>
       <c r="J10" s="15"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="14"/>
+      <c r="K10" s="16">
+        <v>0</v>
+      </c>
+      <c r="L10" s="14">
+        <v>0</v>
+      </c>
       <c r="M10" s="14"/>
     </row>
     <row r="11" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="12">
         <v>7</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="14"/>
+      <c r="B11" s="13">
+        <v>0</v>
+      </c>
+      <c r="C11" s="14">
+        <v>0</v>
+      </c>
       <c r="D11" s="15"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="14"/>
+      <c r="E11" s="16">
+        <v>0</v>
+      </c>
+      <c r="F11" s="14">
+        <v>0</v>
+      </c>
       <c r="G11" s="15"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="14"/>
+      <c r="H11" s="16">
+        <v>0</v>
+      </c>
+      <c r="I11" s="14">
+        <v>0</v>
+      </c>
       <c r="J11" s="15"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="14"/>
+      <c r="K11" s="16">
+        <v>0</v>
+      </c>
+      <c r="L11" s="14">
+        <v>0</v>
+      </c>
       <c r="M11" s="14"/>
     </row>
     <row r="12" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="12">
         <v>8</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
+      <c r="B12" s="13">
+        <v>0</v>
+      </c>
+      <c r="C12" s="14">
+        <v>0</v>
+      </c>
+      <c r="D12" s="15">
+        <v>0</v>
+      </c>
+      <c r="E12" s="16">
+        <v>0</v>
+      </c>
+      <c r="F12" s="14">
+        <v>0</v>
+      </c>
+      <c r="G12" s="15">
+        <v>0</v>
+      </c>
+      <c r="H12" s="16">
+        <v>0</v>
+      </c>
+      <c r="I12" s="14">
+        <v>0</v>
+      </c>
+      <c r="J12" s="15">
+        <v>0</v>
+      </c>
+      <c r="K12" s="16">
+        <v>0</v>
+      </c>
+      <c r="L12" s="14">
+        <v>0</v>
+      </c>
+      <c r="M12" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="12">
         <v>9</v>
       </c>
       <c r="B13" s="13"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="15"/>
+      <c r="C13" s="14">
+        <v>0</v>
+      </c>
+      <c r="D13" s="15">
+        <v>0</v>
+      </c>
       <c r="E13" s="16"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="15"/>
+      <c r="F13" s="14">
+        <v>0</v>
+      </c>
+      <c r="G13" s="15">
+        <v>0</v>
+      </c>
       <c r="H13" s="16"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="15"/>
+      <c r="I13" s="14">
+        <v>0</v>
+      </c>
+      <c r="J13" s="15">
+        <v>0</v>
+      </c>
       <c r="K13" s="16"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
+      <c r="L13" s="14">
+        <v>0</v>
+      </c>
+      <c r="M13" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="12">
         <v>10</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="14"/>
+      <c r="B14" s="13">
+        <v>0</v>
+      </c>
+      <c r="C14" s="14">
+        <v>0</v>
+      </c>
       <c r="D14" s="15"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="14"/>
+      <c r="E14" s="16">
+        <v>0</v>
+      </c>
+      <c r="F14" s="14">
+        <v>0</v>
+      </c>
       <c r="G14" s="15"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="14"/>
+      <c r="H14" s="16">
+        <v>0</v>
+      </c>
+      <c r="I14" s="14">
+        <v>0</v>
+      </c>
       <c r="J14" s="15"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="14"/>
+      <c r="K14" s="16">
+        <v>0</v>
+      </c>
+      <c r="L14" s="14">
+        <v>0</v>
+      </c>
       <c r="M14" s="14"/>
     </row>
     <row r="15" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="12">
         <v>11</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="14"/>
+      <c r="B15" s="13">
+        <v>0</v>
+      </c>
+      <c r="C15" s="14">
+        <v>0</v>
+      </c>
       <c r="D15" s="15"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="14"/>
+      <c r="E15" s="16">
+        <v>0</v>
+      </c>
+      <c r="F15" s="14">
+        <v>0</v>
+      </c>
       <c r="G15" s="15"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="14"/>
+      <c r="H15" s="16">
+        <v>0</v>
+      </c>
+      <c r="I15" s="14">
+        <v>0</v>
+      </c>
       <c r="J15" s="15"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="14"/>
+      <c r="K15" s="16">
+        <v>0</v>
+      </c>
+      <c r="L15" s="14">
+        <v>0</v>
+      </c>
       <c r="M15" s="14"/>
     </row>
     <row r="16" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="12">
         <v>12</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="14"/>
+      <c r="B16" s="13">
+        <v>0</v>
+      </c>
+      <c r="C16" s="14">
+        <v>0</v>
+      </c>
       <c r="D16" s="15"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="14"/>
+      <c r="E16" s="16">
+        <v>0</v>
+      </c>
+      <c r="F16" s="14">
+        <v>0</v>
+      </c>
       <c r="G16" s="15"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="14"/>
+      <c r="H16" s="16">
+        <v>0</v>
+      </c>
+      <c r="I16" s="14">
+        <v>0</v>
+      </c>
       <c r="J16" s="15"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="14"/>
+      <c r="K16" s="16">
+        <v>0</v>
+      </c>
+      <c r="L16" s="14">
+        <v>0</v>
+      </c>
       <c r="M16" s="14"/>
     </row>
     <row r="17" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="12">
         <v>13</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="14"/>
+      <c r="B17" s="13">
+        <v>0</v>
+      </c>
+      <c r="C17" s="14">
+        <v>0</v>
+      </c>
       <c r="D17" s="15"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="14"/>
+      <c r="E17" s="16">
+        <v>0</v>
+      </c>
+      <c r="F17" s="14">
+        <v>0</v>
+      </c>
       <c r="G17" s="15"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="14"/>
+      <c r="H17" s="16">
+        <v>0</v>
+      </c>
+      <c r="I17" s="14">
+        <v>0</v>
+      </c>
       <c r="J17" s="15"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="14"/>
+      <c r="K17" s="16">
+        <v>0</v>
+      </c>
+      <c r="L17" s="14">
+        <v>0</v>
+      </c>
       <c r="M17" s="14"/>
     </row>
     <row r="18" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -6807,67 +7055,131 @@
         <v>14</v>
       </c>
       <c r="B18" s="13"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="15"/>
+      <c r="C18" s="14">
+        <v>0</v>
+      </c>
+      <c r="D18" s="15">
+        <v>0</v>
+      </c>
       <c r="E18" s="16"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="15"/>
+      <c r="F18" s="14">
+        <v>0</v>
+      </c>
+      <c r="G18" s="15">
+        <v>0</v>
+      </c>
       <c r="H18" s="16"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="15"/>
+      <c r="I18" s="14">
+        <v>0</v>
+      </c>
+      <c r="J18" s="15">
+        <v>0</v>
+      </c>
       <c r="K18" s="16"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
+      <c r="L18" s="14">
+        <v>0</v>
+      </c>
+      <c r="M18" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="12">
         <v>15</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="14"/>
+      <c r="B19" s="13">
+        <v>0</v>
+      </c>
+      <c r="C19" s="14">
+        <v>0</v>
+      </c>
       <c r="D19" s="15"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="14"/>
+      <c r="E19" s="16">
+        <v>0</v>
+      </c>
+      <c r="F19" s="14">
+        <v>0</v>
+      </c>
       <c r="G19" s="15"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="14"/>
+      <c r="H19" s="16">
+        <v>0</v>
+      </c>
+      <c r="I19" s="14">
+        <v>0</v>
+      </c>
       <c r="J19" s="15"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="14"/>
+      <c r="K19" s="16">
+        <v>0</v>
+      </c>
+      <c r="L19" s="14">
+        <v>0</v>
+      </c>
       <c r="M19" s="14"/>
     </row>
     <row r="20" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="12">
         <v>16</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="14"/>
+      <c r="B20" s="13">
+        <v>0</v>
+      </c>
+      <c r="C20" s="14">
+        <v>0</v>
+      </c>
       <c r="D20" s="15"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="14"/>
+      <c r="E20" s="16">
+        <v>0</v>
+      </c>
+      <c r="F20" s="14">
+        <v>0</v>
+      </c>
       <c r="G20" s="15"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="14"/>
+      <c r="H20" s="16">
+        <v>0</v>
+      </c>
+      <c r="I20" s="14">
+        <v>0</v>
+      </c>
       <c r="J20" s="15"/>
-      <c r="K20" s="16"/>
-      <c r="L20" s="14"/>
+      <c r="K20" s="16">
+        <v>0</v>
+      </c>
+      <c r="L20" s="14">
+        <v>0</v>
+      </c>
       <c r="M20" s="14"/>
     </row>
     <row r="21" spans="1:13" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="17">
         <v>17</v>
       </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="19"/>
+      <c r="B21" s="18">
+        <v>0</v>
+      </c>
+      <c r="C21" s="19">
+        <v>0</v>
+      </c>
       <c r="D21" s="20"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="19"/>
+      <c r="E21" s="21">
+        <v>0</v>
+      </c>
+      <c r="F21" s="19">
+        <v>0</v>
+      </c>
       <c r="G21" s="20"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="19"/>
+      <c r="H21" s="21">
+        <v>0</v>
+      </c>
+      <c r="I21" s="19">
+        <v>0</v>
+      </c>
       <c r="J21" s="20"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="19"/>
+      <c r="K21" s="21">
+        <v>0</v>
+      </c>
+      <c r="L21" s="19">
+        <v>0</v>
+      </c>
       <c r="M21" s="19"/>
     </row>
   </sheetData>
@@ -6893,11 +7205,11 @@
   </sheetPr>
   <dimension ref="A1:P104"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
strategy test iteration 4 player 0
</commit_message>
<xml_diff>
--- a/tests/src/blueprint/human strategy.xlsx
+++ b/tests/src/blueprint/human strategy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marzukrashid/Downloads/fishbait/fishbait/tests/src/blueprint/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639EBAC5-474A-9446-BFBA-E4AE346B18A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD68996-8706-E34A-BD07-BBE636A9B00B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="regrets" sheetId="1" r:id="rId1"/>
@@ -2045,11 +2045,11 @@
   </sheetPr>
   <dimension ref="A1:U104"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2177,14 +2177,14 @@
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="46"/>
-      <c r="G3" s="41">
-        <v>0</v>
-      </c>
-      <c r="H3" s="28">
-        <v>0</v>
-      </c>
-      <c r="I3" s="28">
-        <v>0</v>
+      <c r="G3" s="64">
+        <v>-4983</v>
+      </c>
+      <c r="H3" s="65">
+        <v>17</v>
+      </c>
+      <c r="I3" s="65">
+        <v>4967</v>
       </c>
       <c r="J3" s="9"/>
       <c r="K3" s="46"/>
@@ -2739,11 +2739,11 @@
       <c r="D16" s="31"/>
       <c r="E16" s="14"/>
       <c r="F16" s="47"/>
-      <c r="G16" s="42">
-        <v>0</v>
-      </c>
-      <c r="H16" s="31">
-        <v>0</v>
+      <c r="G16" s="60">
+        <v>-10050</v>
+      </c>
+      <c r="H16" s="61">
+        <v>10050</v>
       </c>
       <c r="I16" s="31"/>
       <c r="J16" s="14"/>
@@ -7205,11 +7205,11 @@
   </sheetPr>
   <dimension ref="A1:P104"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
strategy test iteration 4 player 1 update strategy
</commit_message>
<xml_diff>
--- a/tests/src/blueprint/human strategy.xlsx
+++ b/tests/src/blueprint/human strategy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marzukrashid/Downloads/fishbait/fishbait/tests/src/blueprint/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD68996-8706-E34A-BD07-BBE636A9B00B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A312F7C5-D7A6-4440-81E5-BF03774066DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="regrets" sheetId="1" r:id="rId1"/>
@@ -654,7 +654,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -882,6 +882,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2045,11 +2051,11 @@
   </sheetPr>
   <dimension ref="A1:U104"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J12" sqref="J12"/>
+      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6470,11 +6476,11 @@
   </sheetPr>
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K5" sqref="K5"/>
+      <selection pane="bottomRight" activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6595,7 +6601,7 @@
       <c r="J4" s="10">
         <v>0</v>
       </c>
-      <c r="K4" s="11">
+      <c r="K4" s="77">
         <v>1</v>
       </c>
       <c r="L4" s="9">
@@ -6618,8 +6624,8 @@
       <c r="D5" s="15">
         <v>0</v>
       </c>
-      <c r="E5" s="16">
-        <v>0</v>
+      <c r="E5" s="76">
+        <v>1</v>
       </c>
       <c r="F5" s="14">
         <v>0</v>
@@ -6756,8 +6762,8 @@
         <v>0</v>
       </c>
       <c r="D9" s="15"/>
-      <c r="E9" s="16">
-        <v>0</v>
+      <c r="E9" s="76">
+        <v>1</v>
       </c>
       <c r="F9" s="14">
         <v>0</v>
@@ -6860,8 +6866,8 @@
       <c r="E12" s="16">
         <v>0</v>
       </c>
-      <c r="F12" s="14">
-        <v>0</v>
+      <c r="F12" s="62">
+        <v>1</v>
       </c>
       <c r="G12" s="15">
         <v>0</v>
@@ -7209,7 +7215,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
strategy test iteration 4 player 2 update strategy
</commit_message>
<xml_diff>
--- a/tests/src/blueprint/human strategy.xlsx
+++ b/tests/src/blueprint/human strategy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marzukrashid/Downloads/fishbait/fishbait/tests/src/blueprint/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A312F7C5-D7A6-4440-81E5-BF03774066DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0D4A29-83D8-0B4B-8014-DB64D65E53C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="regrets" sheetId="1" r:id="rId1"/>
@@ -862,6 +862,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -882,12 +888,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2052,10 +2052,10 @@
   <dimension ref="A1:U104"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="L3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
+      <selection pane="bottomRight" activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2074,34 +2074,34 @@
   <sheetData>
     <row r="1" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2"/>
-      <c r="B1" s="69">
-        <v>0</v>
-      </c>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="72">
-        <v>1</v>
-      </c>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="72">
-        <v>2</v>
-      </c>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="71"/>
-      <c r="Q1" s="72">
+      <c r="B1" s="71">
+        <v>0</v>
+      </c>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="74">
+        <v>1</v>
+      </c>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="74">
+        <v>2</v>
+      </c>
+      <c r="M1" s="72"/>
+      <c r="N1" s="72"/>
+      <c r="O1" s="72"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="74">
         <v>3</v>
       </c>
-      <c r="R1" s="70"/>
-      <c r="S1" s="70"/>
-      <c r="T1" s="70"/>
-      <c r="U1" s="71"/>
+      <c r="R1" s="72"/>
+      <c r="S1" s="72"/>
+      <c r="T1" s="72"/>
+      <c r="U1" s="73"/>
     </row>
     <row r="2" spans="1:21" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
@@ -6480,7 +6480,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I8" sqref="I8"/>
+      <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6490,44 +6490,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="73" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
+      <c r="A1" s="75" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="75"/>
     </row>
     <row r="2" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3"/>
-      <c r="B2" s="69">
-        <v>0</v>
-      </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="75">
-        <v>1</v>
-      </c>
-      <c r="F2" s="70"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="75">
-        <v>2</v>
-      </c>
-      <c r="I2" s="70"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="75">
+      <c r="B2" s="71">
+        <v>0</v>
+      </c>
+      <c r="C2" s="72"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="77">
+        <v>1</v>
+      </c>
+      <c r="F2" s="72"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="77">
+        <v>2</v>
+      </c>
+      <c r="I2" s="72"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="77">
         <v>3</v>
       </c>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
     </row>
     <row r="3" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
@@ -6601,7 +6601,7 @@
       <c r="J4" s="10">
         <v>0</v>
       </c>
-      <c r="K4" s="77">
+      <c r="K4" s="70">
         <v>1</v>
       </c>
       <c r="L4" s="9">
@@ -6624,7 +6624,7 @@
       <c r="D5" s="15">
         <v>0</v>
       </c>
-      <c r="E5" s="76">
+      <c r="E5" s="69">
         <v>1</v>
       </c>
       <c r="F5" s="14">
@@ -6680,8 +6680,8 @@
       <c r="K6" s="16">
         <v>0</v>
       </c>
-      <c r="L6" s="14">
-        <v>0</v>
+      <c r="L6" s="62">
+        <v>1</v>
       </c>
       <c r="M6" s="14"/>
     </row>
@@ -6711,8 +6711,8 @@
         <v>0</v>
       </c>
       <c r="K7" s="16"/>
-      <c r="L7" s="14">
-        <v>0</v>
+      <c r="L7" s="62">
+        <v>1</v>
       </c>
       <c r="M7" s="14">
         <v>0</v>
@@ -6762,7 +6762,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="15"/>
-      <c r="E9" s="76">
+      <c r="E9" s="69">
         <v>1</v>
       </c>
       <c r="F9" s="14">
@@ -6809,8 +6809,8 @@
         <v>0</v>
       </c>
       <c r="J10" s="15"/>
-      <c r="K10" s="16">
-        <v>0</v>
+      <c r="K10" s="69">
+        <v>1</v>
       </c>
       <c r="L10" s="14">
         <v>0</v>
@@ -6842,8 +6842,8 @@
         <v>0</v>
       </c>
       <c r="J11" s="15"/>
-      <c r="K11" s="16">
-        <v>0</v>
+      <c r="K11" s="69">
+        <v>1</v>
       </c>
       <c r="L11" s="14">
         <v>0</v>
@@ -6917,8 +6917,8 @@
         <v>0</v>
       </c>
       <c r="K13" s="16"/>
-      <c r="L13" s="14">
-        <v>0</v>
+      <c r="L13" s="62">
+        <v>1</v>
       </c>
       <c r="M13" s="14">
         <v>0</v>
@@ -6982,8 +6982,8 @@
         <v>0</v>
       </c>
       <c r="J15" s="15"/>
-      <c r="K15" s="16">
-        <v>0</v>
+      <c r="K15" s="69">
+        <v>1</v>
       </c>
       <c r="L15" s="14">
         <v>0</v>
@@ -7082,8 +7082,8 @@
         <v>0</v>
       </c>
       <c r="K18" s="16"/>
-      <c r="L18" s="14">
-        <v>0</v>
+      <c r="L18" s="62">
+        <v>1</v>
       </c>
       <c r="M18" s="14">
         <v>0</v>
@@ -7117,7 +7117,7 @@
       <c r="K19" s="16">
         <v>0</v>
       </c>
-      <c r="L19" s="14">
+      <c r="L19" s="62">
         <v>0</v>
       </c>
       <c r="M19" s="14"/>
@@ -7215,7 +7215,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7225,24 +7225,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="73" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="73"/>
-      <c r="O1" s="73"/>
-      <c r="P1" s="73"/>
+      <c r="A1" s="75" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="75"/>
+      <c r="N1" s="75"/>
+      <c r="O1" s="75"/>
+      <c r="P1" s="75"/>
     </row>
     <row r="2" spans="1:16" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">

</xml_diff>

<commit_message>
strategy test iteration 4 player 2
</commit_message>
<xml_diff>
--- a/tests/src/blueprint/human strategy.xlsx
+++ b/tests/src/blueprint/human strategy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marzukrashid/Downloads/fishbait/fishbait/tests/src/blueprint/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0D4A29-83D8-0B4B-8014-DB64D65E53C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A07B3B3-3B97-E148-82EC-17191045766C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="regrets" sheetId="1" r:id="rId1"/>
@@ -2051,11 +2051,11 @@
   </sheetPr>
   <dimension ref="A1:U104"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="L3" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="Q14" sqref="Q14"/>
+      <selection pane="bottomRight" activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2500,11 +2500,11 @@
       <c r="I10" s="31"/>
       <c r="J10" s="14"/>
       <c r="K10" s="47"/>
-      <c r="L10" s="42">
-        <v>0</v>
-      </c>
-      <c r="M10" s="31">
-        <v>0</v>
+      <c r="L10" s="60">
+        <v>4950</v>
+      </c>
+      <c r="M10" s="61">
+        <v>-4950</v>
       </c>
       <c r="N10" s="31"/>
       <c r="O10" s="14"/>
@@ -6476,11 +6476,11 @@
   </sheetPr>
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
+      <selection pane="bottomRight" activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7215,7 +7215,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
strategy test iteration 5 player 1
</commit_message>
<xml_diff>
--- a/tests/src/blueprint/human strategy.xlsx
+++ b/tests/src/blueprint/human strategy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marzukrashid/Downloads/fishbait/fishbait/tests/src/blueprint/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A07B3B3-3B97-E148-82EC-17191045766C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{040E026B-F7EE-5243-83BC-DE968958D8F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="regrets" sheetId="1" r:id="rId1"/>
@@ -2051,11 +2051,11 @@
   </sheetPr>
   <dimension ref="A1:U104"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="N10" sqref="N10"/>
+      <selection pane="bottomRight" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7211,11 +7211,11 @@
   </sheetPr>
   <dimension ref="A1:P104"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
strategy test iteration 5 player 2
</commit_message>
<xml_diff>
--- a/tests/src/blueprint/human strategy.xlsx
+++ b/tests/src/blueprint/human strategy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marzukrashid/Downloads/fishbait/fishbait/tests/src/blueprint/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{040E026B-F7EE-5243-83BC-DE968958D8F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD791E7-119C-9F42-B76D-5ECF375BD8AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="regrets" sheetId="1" r:id="rId1"/>
@@ -2051,11 +2051,11 @@
   </sheetPr>
   <dimension ref="A1:U104"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I4" sqref="I4"/>
+      <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7211,11 +7211,11 @@
   </sheetPr>
   <dimension ref="A1:P104"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>